<commit_message>
automatic bills dowloader 1.1
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -109,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,15 +120,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,10 +365,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -515,6 +539,87 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>160252832341</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>160252832367</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>170743925516</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>170741644315</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>170741644412</v>
+      </c>
+      <c r="B20" s="5">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>170741644404</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>170003628933</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>170003629018</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>170003629026</v>
+      </c>
+      <c r="B24" s="5">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>170003629034</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4745</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
automatic bills downloader 1.2
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Consumer</t>
   </si>
@@ -53,34 +53,25 @@
     <t>oct,nov</t>
   </si>
   <si>
-    <t>jan,mar</t>
-  </si>
-  <si>
-    <t>dec,feb</t>
-  </si>
-  <si>
-    <t>jan,nov</t>
-  </si>
-  <si>
-    <t>sep,may</t>
-  </si>
-  <si>
-    <t>may,apr</t>
-  </si>
-  <si>
-    <t>dec,mar</t>
-  </si>
-  <si>
-    <t>nov,aug</t>
+    <t xml:space="preserve"> jan,mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dec,feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sep,may</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jan,nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> may,apr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -139,15 +130,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -368,13 +362,16 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="7" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -408,7 +405,7 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
+      <c r="A2" s="6">
         <v>170688856348</v>
       </c>
       <c r="B2" s="3">
@@ -419,7 +416,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>170688851621</v>
       </c>
       <c r="B3" s="3">
@@ -430,7 +427,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+      <c r="A4" s="6">
         <v>170688861384</v>
       </c>
       <c r="B4" s="3">
@@ -441,7 +438,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+      <c r="A5" s="6">
         <v>170688858995</v>
       </c>
       <c r="B5" s="3">
@@ -452,7 +449,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
+      <c r="A6" s="6">
         <v>170688852041</v>
       </c>
       <c r="B6" s="3">
@@ -463,7 +460,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+      <c r="A7" s="6">
         <v>170688852075</v>
       </c>
       <c r="B7" s="3">
@@ -474,7 +471,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>170688859011</v>
       </c>
       <c r="B8" s="3">
@@ -485,29 +482,29 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>170675839380</v>
       </c>
       <c r="B9" s="3">
         <v>4636</v>
       </c>
       <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>170688851648</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4636</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
-        <v>170688851648</v>
-      </c>
-      <c r="B10" s="3">
-        <v>4636</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>170688856313</v>
       </c>
       <c r="B11" s="3">
@@ -518,107 +515,53 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
-        <v>170688859029</v>
-      </c>
-      <c r="B12" s="3">
-        <v>4636</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
-        <v>170688852059</v>
-      </c>
-      <c r="B13" s="3">
-        <v>4636</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="6"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>160252832341</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4610</v>
-      </c>
+      <c r="A16" s="8"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>160252832367</v>
-      </c>
-      <c r="B17" s="5">
-        <v>4610</v>
-      </c>
+      <c r="A17" s="8"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>170743925516</v>
-      </c>
-      <c r="B18" s="5">
-        <v>4746</v>
-      </c>
+      <c r="A18" s="8"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>170741644315</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4746</v>
-      </c>
+      <c r="A19" s="8"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>170741644412</v>
-      </c>
-      <c r="B20" s="5">
-        <v>4746</v>
-      </c>
+      <c r="A20" s="8"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>170741644404</v>
-      </c>
-      <c r="B21" s="5">
-        <v>4746</v>
-      </c>
+      <c r="A21" s="8"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>170003628933</v>
-      </c>
-      <c r="B22" s="5">
-        <v>4745</v>
-      </c>
+      <c r="A22" s="8"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>170003629018</v>
-      </c>
-      <c r="B23" s="5">
-        <v>4745</v>
-      </c>
+      <c r="A23" s="8"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>170003629026</v>
-      </c>
-      <c r="B24" s="5">
-        <v>4745</v>
-      </c>
+      <c r="A24" s="8"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>170003629034</v>
-      </c>
-      <c r="B25" s="5">
-        <v>4745</v>
-      </c>
+      <c r="A25" s="8"/>
+      <c r="B25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>